<commit_message>
Added command to run and view
</commit_message>
<xml_diff>
--- a/utils/Client_5_nintendo.xlsx
+++ b/utils/Client_5_nintendo.xlsx
@@ -41,7 +41,7 @@
     <t xml:space="preserve">6x0UW2uwT%</t>
   </si>
   <si>
-    <t xml:space="preserve">qanintendo.dsidrm.com</t>
+    <t xml:space="preserve">https://qanintendo.dsidrm.com</t>
   </si>
   <si>
     <t xml:space="preserve">companyName</t>
@@ -440,7 +440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -452,6 +452,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://qanintendo"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -554,7 +557,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.21"/>
@@ -644,7 +647,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.33"/>
@@ -716,7 +719,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.0078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="22.015625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.33"/>

</xml_diff>